<commit_message>
temperature の harmonized name を temp から temperature に変更、分かりやすくするため
</commit_message>
<xml_diff>
--- a/ykodama/ddbj_packages/excel/Beta-lactamase.1.0.xlsx
+++ b/ykodama/ddbj_packages/excel/Beta-lactamase.1.0.xlsx
@@ -164,12 +164,103 @@
         </r>
       </text>
     </comment>
+    <comment ref="L15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of persons or institute who collected the sample</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time of sampling (single instance or interval, eg., 2008-01-23T19:23:10, 2008-01-23, 2008-01, 2008, 1952-10-21T11:43Z/1952-10-21T17:43Z, 1952-10-21/1953-02-15, 1952-10/1953-02, 1952/1953)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Geographical origin of the sample; use the appropriate name from the list, http://www.ddbj.nig.ac.jp/sub/country-e.html. Use a colon to separate the country or ocean from more detailed information about the location, eg "Japan:Kanagawa, Hakone, Lake Ashi" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The natural (as opposed to laboratory) host to the organism from which the sample was obtained. Use the full taxonomic name, eg, "Homo sapiens".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Describes the physical, environmental and/or local geographical source of the biological sample from which the sample was derived.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scientific name and description of the laboratory host used to propagate the source organism or material from which the sample was obtained, e.g., Escherichia coli DH5a, or Homo sapiens HeLa cells</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The geographical coordinates of the location where the sample was collected. Specify as decimal degrees latitude and longitude in format "d[d.dddd] N|S d[dd.dddd] W|E", eg, 47.94 N 28.12 W</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve"># This is a submission template for batch deposit of 'Beta-lactamase; version 1.0' samples to the DDBJ BioSample database (http://trace.ddbj.nig.ac.jp/biosample)._x000D_
 </t>
@@ -258,6 +349,27 @@
   </si>
   <si>
     <t>edta_inhibitor_tested</t>
+  </si>
+  <si>
+    <t>collected_by</t>
+  </si>
+  <si>
+    <t>collection_date</t>
+  </si>
+  <si>
+    <t>geo_loc_name</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>isolation_source</t>
+  </si>
+  <si>
+    <t>lab_host</t>
+  </si>
+  <si>
+    <t>lat_lon</t>
   </si>
 </sst>
 </file>
@@ -678,77 +790,77 @@
     <col min="1" max="201" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1">
+    <row r="3" spans="1:18" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1">
+    <row r="4" spans="1:18" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1">
+    <row r="5" spans="1:18" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:18">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:18">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:18">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:18">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:18">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:18">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:18">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:18">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:18">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -781,6 +893,27 @@
       </c>
       <c r="K15" s="7" t="s">
         <v>24</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>